<commit_message>
adding date of birth to service uptake export
</commit_message>
<xml_diff>
--- a/templates/excel_template/service_uptake_template.xlsx
+++ b/templates/excel_template/service_uptake_template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antonyojwang/Documents/Work/Dreams/service_uptake_export/template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antonyojwang/myprojects/pythonProjects/dreams-database/templates/excel_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="3680" windowWidth="26160" windowHeight="14380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15520" windowHeight="24000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="DREAMS_Services" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
     <t>IP_NAME</t>
   </si>
   <si>
-    <t>IP_CODE</t>
-  </si>
-  <si>
     <t>date_given</t>
   </si>
   <si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>Ward</t>
+  </si>
+  <si>
+    <t>DOB</t>
   </si>
 </sst>
 </file>
@@ -418,49 +418,49 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>5</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>6</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>7</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding date of enrollment to raw service uptake
</commit_message>
<xml_diff>
--- a/templates/excel_template/service_uptake_template.xlsx
+++ b/templates/excel_template/service_uptake_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15520" windowHeight="24000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="15520" windowHeight="22320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="DREAMS_Services" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>client_id</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>DOB</t>
+  </si>
+  <si>
+    <t>Date_of_enrollment</t>
   </si>
 </sst>
 </file>
@@ -392,25 +395,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.1640625" customWidth="1"/>
-    <col min="2" max="8" width="14.83203125" customWidth="1"/>
-    <col min="9" max="9" width="15.83203125" customWidth="1"/>
-    <col min="10" max="10" width="21.83203125" customWidth="1"/>
-    <col min="11" max="11" width="25.33203125" customWidth="1"/>
-    <col min="12" max="12" width="16.6640625" customWidth="1"/>
-    <col min="13" max="13" width="26.83203125" customWidth="1"/>
-    <col min="14" max="15" width="19.6640625" customWidth="1"/>
-    <col min="16" max="16" width="22.5" customWidth="1"/>
-    <col min="17" max="17" width="19.6640625" customWidth="1"/>
+    <col min="2" max="5" width="14.83203125" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" customWidth="1"/>
+    <col min="7" max="9" width="14.83203125" customWidth="1"/>
+    <col min="10" max="10" width="15.83203125" customWidth="1"/>
+    <col min="11" max="11" width="21.83203125" customWidth="1"/>
+    <col min="12" max="12" width="25.33203125" customWidth="1"/>
+    <col min="13" max="13" width="16.6640625" customWidth="1"/>
+    <col min="14" max="14" width="26.83203125" customWidth="1"/>
+    <col min="15" max="16" width="19.6640625" customWidth="1"/>
+    <col min="17" max="17" width="22.5" customWidth="1"/>
+    <col min="18" max="18" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -427,39 +434,42 @@
         <v>16</v>
       </c>
       <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>4</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>5</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added village to service uptake raw export
</commit_message>
<xml_diff>
--- a/templates/excel_template/service_uptake_template.xlsx
+++ b/templates/excel_template/service_uptake_template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>client_id</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Date_of_enrollment</t>
+  </si>
+  <si>
+    <t>Village</t>
   </si>
 </sst>
 </file>
@@ -395,29 +398,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.1640625" customWidth="1"/>
     <col min="2" max="5" width="14.83203125" customWidth="1"/>
     <col min="6" max="6" width="17.83203125" customWidth="1"/>
-    <col min="7" max="9" width="14.83203125" customWidth="1"/>
-    <col min="10" max="10" width="15.83203125" customWidth="1"/>
-    <col min="11" max="11" width="21.83203125" customWidth="1"/>
-    <col min="12" max="12" width="25.33203125" customWidth="1"/>
-    <col min="13" max="13" width="16.6640625" customWidth="1"/>
-    <col min="14" max="14" width="26.83203125" customWidth="1"/>
-    <col min="15" max="16" width="19.6640625" customWidth="1"/>
-    <col min="17" max="17" width="22.5" customWidth="1"/>
-    <col min="18" max="18" width="19.6640625" customWidth="1"/>
+    <col min="7" max="10" width="14.83203125" customWidth="1"/>
+    <col min="11" max="11" width="15.83203125" customWidth="1"/>
+    <col min="12" max="12" width="21.83203125" customWidth="1"/>
+    <col min="13" max="13" width="25.33203125" customWidth="1"/>
+    <col min="14" max="14" width="16.6640625" customWidth="1"/>
+    <col min="15" max="15" width="26.83203125" customWidth="1"/>
+    <col min="16" max="17" width="19.6640625" customWidth="1"/>
+    <col min="18" max="18" width="22.5" customWidth="1"/>
+    <col min="19" max="19" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -446,30 +447,33 @@
         <v>15</v>
       </c>
       <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
         <v>3</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>4</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>6</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added current_age and age at intervention to raw interventions export. Also restricted access to PHI column in raw intervention export
</commit_message>
<xml_diff>
--- a/templates/excel_template/service_uptake_template.xlsx
+++ b/templates/excel_template/service_uptake_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="15520" windowHeight="22320" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="DREAMS_Services" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>client_id</t>
   </si>
@@ -84,6 +84,12 @@
   </si>
   <si>
     <t>Village</t>
+  </si>
+  <si>
+    <t>age_at_intervention</t>
+  </si>
+  <si>
+    <t>current_age</t>
   </si>
 </sst>
 </file>
@@ -398,9 +404,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -409,16 +417,18 @@
     <col min="6" max="6" width="17.83203125" customWidth="1"/>
     <col min="7" max="10" width="14.83203125" customWidth="1"/>
     <col min="11" max="11" width="15.83203125" customWidth="1"/>
-    <col min="12" max="12" width="21.83203125" customWidth="1"/>
-    <col min="13" max="13" width="25.33203125" customWidth="1"/>
-    <col min="14" max="14" width="16.6640625" customWidth="1"/>
-    <col min="15" max="15" width="26.83203125" customWidth="1"/>
-    <col min="16" max="17" width="19.6640625" customWidth="1"/>
-    <col min="18" max="18" width="22.5" customWidth="1"/>
-    <col min="19" max="19" width="19.6640625" customWidth="1"/>
+    <col min="12" max="12" width="17.83203125" customWidth="1"/>
+    <col min="13" max="13" width="15.83203125" customWidth="1"/>
+    <col min="14" max="14" width="21.83203125" customWidth="1"/>
+    <col min="15" max="15" width="25.33203125" customWidth="1"/>
+    <col min="16" max="16" width="16.6640625" customWidth="1"/>
+    <col min="17" max="17" width="26.83203125" customWidth="1"/>
+    <col min="18" max="19" width="19.6640625" customWidth="1"/>
+    <col min="20" max="20" width="22.5" customWidth="1"/>
+    <col min="21" max="21" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -453,27 +463,33 @@
         <v>3</v>
       </c>
       <c r="L1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>5</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>6</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>